<commit_message>
updated emissions intensity data
</commit_message>
<xml_diff>
--- a/data-raw/external_data/AEMO/emissions-intensity-grid.xlsx
+++ b/data-raw/external_data/AEMO/emissions-intensity-grid.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lffox/Dropbox (Grattan Institute)/Transport Program/Project - Electric vehicles/Analysis/efficiency-standards-analysis/cba-standards/cba-standards/data/AEMO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lffox/Dropbox (Grattan Institute)/Transport Program/Project - Electric vehicles/Analysis/fleeteffSim/data-raw/external_data/AEMO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091ED12F-B3DF-4943-AAFF-CEA4CEAA98D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2C1A33-4C6D-ED47-998A-35CF372E5564}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-8940" windowWidth="38400" windowHeight="21600" xr2:uid="{CE561C37-8DAE-D84D-B965-64D293181412}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{CE561C37-8DAE-D84D-B965-64D293181412}"/>
   </bookViews>
   <sheets>
     <sheet name="step_change" sheetId="1" r:id="rId1"/>
     <sheet name="notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>data is taken from isp scenario (step change DSP4) and calculated based on the total emissions/electricity</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>EI(g_wh)</t>
+  </si>
+  <si>
+    <t>old</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D30E987-2986-4A40-8EE4-C9D441442941}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,6 +431,9 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -438,6 +444,9 @@
       <c r="B2">
         <v>0.31791892903202085</v>
       </c>
+      <c r="C2">
+        <v>0.62422682874642976</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -446,6 +455,9 @@
       <c r="B3">
         <v>0.28823920010027443</v>
       </c>
+      <c r="C3">
+        <v>0.61939975050351725</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -454,6 +466,9 @@
       <c r="B4">
         <v>0.25916309862000697</v>
       </c>
+      <c r="C4">
+        <v>0.61540940649038212</v>
+      </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -463,6 +478,9 @@
       <c r="B5">
         <v>0.23056502455523664</v>
       </c>
+      <c r="C5">
+        <v>0.59871070537004722</v>
+      </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -472,6 +490,9 @@
       <c r="B6">
         <v>0.20260996592015151</v>
       </c>
+      <c r="C6">
+        <v>0.58387019051458278</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -481,6 +502,9 @@
       <c r="B7">
         <v>0.17569456607195677</v>
       </c>
+      <c r="C7">
+        <v>0.55465722631191772</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -490,6 +514,9 @@
       <c r="B8">
         <v>0.15188792329922635</v>
       </c>
+      <c r="C8">
+        <v>0.57214187305195952</v>
+      </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -499,6 +526,9 @@
       <c r="B9">
         <v>0.13119881176919604</v>
       </c>
+      <c r="C9">
+        <v>0.51823856546817315</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -508,6 +538,9 @@
       <c r="B10">
         <v>0.11211820883275055</v>
       </c>
+      <c r="C10">
+        <v>0.4997748244352076</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -517,6 +550,9 @@
       <c r="B11">
         <v>9.4554615142264292E-2</v>
       </c>
+      <c r="C11">
+        <v>0.50539883731315405</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -526,6 +562,9 @@
       <c r="B12">
         <v>7.7644642755889406E-2</v>
       </c>
+      <c r="C12">
+        <v>0.46637253828755709</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -535,6 +574,9 @@
       <c r="B13">
         <v>6.5919060481575809E-2</v>
       </c>
+      <c r="C13">
+        <v>0.41443359671112523</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -544,6 +586,9 @@
       <c r="B14">
         <v>5.6080547188546097E-2</v>
       </c>
+      <c r="C14">
+        <v>0.41600911249874645</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -553,6 +598,9 @@
       <c r="B15">
         <v>4.8359089898088702E-2</v>
       </c>
+      <c r="C15">
+        <v>0.40469834416909695</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -562,6 +610,9 @@
       <c r="B16">
         <v>3.9900005755151409E-2</v>
       </c>
+      <c r="C16">
+        <v>0.30850420341150847</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -571,6 +622,9 @@
       <c r="B17">
         <v>3.0867100535907466E-2</v>
       </c>
+      <c r="C17">
+        <v>0.27989452129631548</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -580,6 +634,9 @@
       <c r="B18">
         <v>2.7178884543493424E-2</v>
       </c>
+      <c r="C18">
+        <v>0.25264010087669825</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -589,6 +646,9 @@
       <c r="B19">
         <v>2.5480099560302647E-2</v>
       </c>
+      <c r="C19">
+        <v>0.24722333414421613</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -598,6 +658,9 @@
       <c r="B20">
         <v>2.3102829107084551E-2</v>
       </c>
+      <c r="C20">
+        <v>0.24841309236874204</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -607,6 +670,9 @@
       <c r="B21">
         <v>2.0947160914387138E-2</v>
       </c>
+      <c r="C21">
+        <v>0.24474313158762934</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -616,6 +682,9 @@
       <c r="B22">
         <v>1.8492643316397328E-2</v>
       </c>
+      <c r="C22">
+        <v>0.23062618419074904</v>
+      </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -625,6 +694,9 @@
       <c r="B23" s="2">
         <v>1.512818745164725E-2</v>
       </c>
+      <c r="C23" s="2">
+        <v>0.20500105261399915</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -634,6 +706,9 @@
       <c r="B24" s="2">
         <v>1.3237164020191341E-2</v>
       </c>
+      <c r="C24" s="2">
+        <v>0.17937592103724925</v>
+      </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -643,6 +718,9 @@
       <c r="B25" s="2">
         <v>1.1346140588735438E-2</v>
       </c>
+      <c r="C25" s="2">
+        <v>0.15375078946049936</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
@@ -651,6 +729,9 @@
       <c r="B26" s="2">
         <v>9.4551171572795304E-3</v>
       </c>
+      <c r="C26" s="2">
+        <v>0.12812565788374947</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
@@ -659,6 +740,9 @@
       <c r="B27" s="2">
         <v>7.5640937258236226E-3</v>
       </c>
+      <c r="C27" s="2">
+        <v>0.10250052630699957</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
@@ -667,6 +751,9 @@
       <c r="B28" s="2">
         <v>5.6730702943677182E-3</v>
       </c>
+      <c r="C28" s="2">
+        <v>7.687539473024968E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
@@ -675,6 +762,9 @@
       <c r="B29" s="2">
         <v>3.7820468629118122E-3</v>
       </c>
+      <c r="C29" s="2">
+        <v>5.1250263153499787E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
@@ -683,6 +773,9 @@
       <c r="B30" s="2">
         <v>1.8910234314559061E-3</v>
       </c>
+      <c r="C30" s="2">
+        <v>2.5625131576749893E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
@@ -691,6 +784,12 @@
       <c r="B31" s="2">
         <v>0</v>
       </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -701,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F81B1A-2C11-824F-AACE-3C3CE7280E9A}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated fuel costs and emissions of grid
</commit_message>
<xml_diff>
--- a/data-raw/external_data/AEMO/emissions-intensity-grid.xlsx
+++ b/data-raw/external_data/AEMO/emissions-intensity-grid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lffox/Dropbox (Grattan Institute)/Transport Program/Project - Electric vehicles/Analysis/fleeteffSim/data-raw/external_data/AEMO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2C1A33-4C6D-ED47-998A-35CF372E5564}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92432B7E-D6BD-814E-A25D-33AFCD70ABFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{CE561C37-8DAE-D84D-B965-64D293181412}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21020" xr2:uid="{CE561C37-8DAE-D84D-B965-64D293181412}"/>
   </bookViews>
   <sheets>
     <sheet name="step_change" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>data is taken from isp scenario (step change DSP4) and calculated based on the total emissions/electricity</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>old</t>
+  </si>
+  <si>
+    <t>step_change</t>
   </si>
 </sst>
 </file>
@@ -66,10 +69,9 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -95,18 +97,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -418,378 +421,474 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D30E987-2986-4A40-8EE4-C9D441442941}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:Y32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="10.83203125" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2021</v>
       </c>
-      <c r="B2">
-        <v>0.31791892903202085</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="3">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="C2" s="4">
         <v>0.62422682874642976</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="4">
+        <v>0.64236732473407676</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2022</v>
       </c>
-      <c r="B3">
-        <v>0.28823920010027443</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="3">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="C3" s="4">
         <v>0.61939975050351725</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="4">
+        <v>0.61177840450864451</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2023</v>
       </c>
-      <c r="B4">
-        <v>0.25916309862000697</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="3">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="C4" s="4">
         <v>0.61540940649038212</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="4">
+        <v>0.59843580933578844</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2024</v>
       </c>
-      <c r="B5">
-        <v>0.23056502455523664</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="3">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="C5" s="4">
         <v>0.59871070537004722</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="4">
+        <v>0.58179345387917392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2025</v>
       </c>
-      <c r="B6">
-        <v>0.20260996592015151</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="3">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="C6" s="4">
         <v>0.58387019051458278</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="4">
+        <v>0.55721823127845405</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2026</v>
       </c>
-      <c r="B7">
-        <v>0.17569456607195677</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="3">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="C7" s="4">
         <v>0.55465722631191772</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="4">
+        <v>0.49126104290625566</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2027</v>
       </c>
-      <c r="B8">
-        <v>0.15188792329922635</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="3">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="C8" s="4">
         <v>0.57214187305195952</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="4">
+        <v>0.42512837118934171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2028</v>
       </c>
-      <c r="B9">
-        <v>0.13119881176919604</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="3">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="C9" s="4">
         <v>0.51823856546817315</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="4">
+        <v>0.38917615245473314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2029</v>
       </c>
-      <c r="B10">
-        <v>0.11211820883275055</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="3">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="C10" s="4">
         <v>0.4997748244352076</v>
       </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="4">
+        <v>0.35505392067263752</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2030</v>
       </c>
-      <c r="B11">
-        <v>9.4554615142264292E-2</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C11" s="4">
         <v>0.50539883731315405</v>
       </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="4">
+        <v>0.3381994477274976</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2031</v>
       </c>
-      <c r="B12">
-        <v>7.7644642755889406E-2</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="3">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="C12" s="4">
         <v>0.46637253828755709</v>
       </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="4">
+        <v>0.30043070596784771</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2032</v>
       </c>
-      <c r="B13">
-        <v>6.5919060481575809E-2</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="3">
+        <v>0.187</v>
+      </c>
+      <c r="C13" s="4">
         <v>0.41443359671112523</v>
       </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" s="4">
+        <v>0.24301229975611041</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2033</v>
       </c>
-      <c r="B14">
-        <v>5.6080547188546097E-2</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="3">
+        <v>0.184</v>
+      </c>
+      <c r="C14" s="4">
         <v>0.41600911249874645</v>
       </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" s="4">
+        <v>0.1873453211263218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2034</v>
       </c>
-      <c r="B15">
-        <v>4.8359089898088702E-2</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="3">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C15" s="4">
         <v>0.40469834416909695</v>
       </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" s="4">
+        <v>0.18370443618508542</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2035</v>
       </c>
-      <c r="B16">
-        <v>3.9900005755151409E-2</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="3">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C16" s="4">
         <v>0.30850420341150847</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="4">
+        <v>0.17539358404381053</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2036</v>
       </c>
-      <c r="B17">
-        <v>3.0867100535907466E-2</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="3">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="C17" s="4">
         <v>0.27989452129631548</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="4">
+        <v>8.250212442970406E-2</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2037</v>
       </c>
-      <c r="B18">
-        <v>2.7178884543493424E-2</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="3">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="C18" s="4">
         <v>0.25264010087669825</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="4">
+        <v>4.9263089324973537E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2038</v>
       </c>
-      <c r="B19">
-        <v>2.5480099560302647E-2</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="3">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C19" s="4">
         <v>0.24722333414421613</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="4">
+        <v>5.4007344998919855E-2</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2039</v>
       </c>
-      <c r="B20">
-        <v>2.3102829107084551E-2</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="3">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C20" s="4">
         <v>0.24841309236874204</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="4">
+        <v>4.6815179226756064E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2040</v>
       </c>
-      <c r="B21">
-        <v>2.0947160914387138E-2</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="3">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="C21" s="4">
         <v>0.24474313158762934</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="4">
+        <v>4.5492336894285224E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2041</v>
       </c>
-      <c r="B22">
-        <v>1.8492643316397328E-2</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="C22" s="4">
         <v>0.23062618419074904</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="4">
+        <v>4.8772746099148022E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>2042</v>
       </c>
-      <c r="B23" s="2">
-        <v>1.512818745164725E-2</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="B23" s="5">
+        <v>2.6666666666666665E-2</v>
+      </c>
+      <c r="C23" s="5">
         <v>0.20500105261399915</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="4">
+        <v>3.0256374903294497E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>2043</v>
       </c>
-      <c r="B24" s="2">
-        <v>1.3237164020191341E-2</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="B24" s="5">
+        <v>2.3333333333333331E-2</v>
+      </c>
+      <c r="C24" s="5">
         <v>0.17937592103724925</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="4">
+        <v>2.6474328040382685E-2</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>2044</v>
       </c>
-      <c r="B25" s="2">
-        <v>1.1346140588735438E-2</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="B25" s="5">
+        <v>1.9999999999999997E-2</v>
+      </c>
+      <c r="C25" s="5">
         <v>0.15375078946049936</v>
       </c>
+      <c r="D25" s="4">
+        <v>2.2692281177470873E-2</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>2045</v>
       </c>
-      <c r="B26" s="2">
-        <v>9.4551171572795304E-3</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="B26" s="5">
+        <v>1.6666666666666663E-2</v>
+      </c>
+      <c r="C26" s="5">
         <v>0.12812565788374947</v>
       </c>
+      <c r="D26" s="4">
+        <v>1.8910234314559061E-2</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>2046</v>
       </c>
-      <c r="B27" s="2">
-        <v>7.5640937258236226E-3</v>
-      </c>
-      <c r="C27" s="2">
+      <c r="B27" s="5">
+        <v>1.3333333333333329E-2</v>
+      </c>
+      <c r="C27" s="5">
         <v>0.10250052630699957</v>
       </c>
+      <c r="D27" s="4">
+        <v>1.5128187451647249E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>2047</v>
       </c>
-      <c r="B28" s="2">
-        <v>5.6730702943677182E-3</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="B28" s="5">
+        <v>9.999999999999995E-3</v>
+      </c>
+      <c r="C28" s="5">
         <v>7.687539473024968E-2</v>
       </c>
+      <c r="D28" s="4">
+        <v>1.1346140588735436E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>2048</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="5">
+        <v>6.6666666666666619E-3</v>
+      </c>
+      <c r="C29" s="5">
+        <v>5.1250263153499787E-2</v>
+      </c>
+      <c r="D29" s="4">
+        <v>7.5640937258236243E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>2049</v>
+      </c>
+      <c r="B30" s="5">
+        <v>3.3333333333333288E-3</v>
+      </c>
+      <c r="C30" s="5">
+        <v>2.5625131576749893E-2</v>
+      </c>
+      <c r="D30" s="4">
         <v>3.7820468629118122E-3</v>
       </c>
-      <c r="C29" s="2">
-        <v>5.1250263153499787E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>2049</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1.8910234314559061E-3</v>
-      </c>
-      <c r="C30" s="2">
-        <v>2.5625131576749893E-2</v>
-      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>2050</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="5">
         <v>0</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="5">
         <v>0</v>
       </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C32" s="2"/>
+      <c r="C32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated enegry intensity labels
</commit_message>
<xml_diff>
--- a/data-raw/external_data/AEMO/emissions-intensity-grid.xlsx
+++ b/data-raw/external_data/AEMO/emissions-intensity-grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lffox/Dropbox (Grattan Institute)/Transport Program/Project - Electric vehicles/Analysis/fleeteffSim/data-raw/external_data/AEMO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92432B7E-D6BD-814E-A25D-33AFCD70ABFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01991C0-9468-6542-B72A-3D69C0139955}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21020" xr2:uid="{CE561C37-8DAE-D84D-B965-64D293181412}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>data is taken from isp scenario (step change DSP4) and calculated based on the total emissions/electricity</t>
   </si>
@@ -48,17 +48,14 @@
   <si>
     <t>EI(g_wh)</t>
   </si>
-  <si>
-    <t>old</t>
-  </si>
-  <si>
-    <t>step_change</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -100,13 +97,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D30E987-2986-4A40-8EE4-C9D441442941}">
-  <dimension ref="A1:Y32"/>
+  <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="K14" sqref="K14:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,12 +437,6 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3"/>
@@ -471,424 +465,316 @@
       <c r="A2">
         <v>2021</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>0.61199999999999999</v>
       </c>
-      <c r="C2" s="4">
-        <v>0.62422682874642976</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.64236732473407676</v>
-      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2022</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>0.59799999999999998</v>
       </c>
-      <c r="C3" s="4">
-        <v>0.61939975050351725</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.61177840450864451</v>
-      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2023</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>0.58199999999999996</v>
       </c>
-      <c r="C4" s="4">
-        <v>0.61540940649038212</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.59843580933578844</v>
-      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2024</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>0.55700000000000005</v>
       </c>
-      <c r="C5" s="4">
-        <v>0.59871070537004722</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.58179345387917392</v>
-      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2025</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>0.49099999999999999</v>
       </c>
-      <c r="C6" s="4">
-        <v>0.58387019051458278</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.55721823127845405</v>
-      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2026</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>0.42499999999999999</v>
       </c>
-      <c r="C7" s="4">
-        <v>0.55465722631191772</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.49126104290625566</v>
-      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2027</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>0.38900000000000001</v>
       </c>
-      <c r="C8" s="4">
-        <v>0.57214187305195952</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.42512837118934171</v>
-      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2028</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>0.35499999999999998</v>
       </c>
-      <c r="C9" s="4">
-        <v>0.51823856546817315</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.38917615245473314</v>
-      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2029</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>0.33800000000000002</v>
       </c>
-      <c r="C10" s="4">
-        <v>0.4997748244352076</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.35505392067263752</v>
-      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2030</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>0.3</v>
       </c>
-      <c r="C11" s="4">
-        <v>0.50539883731315405</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.3381994477274976</v>
-      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2031</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
         <v>0.24299999999999999</v>
       </c>
-      <c r="C12" s="4">
-        <v>0.46637253828755709</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0.30043070596784771</v>
-      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2032</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="5">
         <v>0.187</v>
       </c>
-      <c r="C13" s="4">
-        <v>0.41443359671112523</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.24301229975611041</v>
-      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2033</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="5">
         <v>0.184</v>
       </c>
-      <c r="C14" s="4">
-        <v>0.41600911249874645</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.1873453211263218</v>
-      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2034</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="5">
         <v>0.17499999999999999</v>
       </c>
-      <c r="C15" s="4">
-        <v>0.40469834416909695</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.18370443618508542</v>
-      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2035</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="5">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="C16" s="4">
-        <v>0.30850420341150847</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.17539358404381053</v>
-      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2036</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="5">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="C17" s="4">
-        <v>0.27989452129631548</v>
-      </c>
-      <c r="D17" s="4">
-        <v>8.250212442970406E-2</v>
-      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2037</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="5">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="C18" s="4">
-        <v>0.25264010087669825</v>
-      </c>
-      <c r="D18" s="4">
-        <v>4.9263089324973537E-2</v>
-      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2038</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="5">
         <v>4.7E-2</v>
       </c>
-      <c r="C19" s="4">
-        <v>0.24722333414421613</v>
-      </c>
-      <c r="D19" s="4">
-        <v>5.4007344998919855E-2</v>
-      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2039</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="5">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C20" s="4">
-        <v>0.24841309236874204</v>
-      </c>
-      <c r="D20" s="4">
-        <v>4.6815179226756064E-2</v>
-      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2040</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="5">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="C21" s="4">
-        <v>0.24474313158762934</v>
-      </c>
-      <c r="D21" s="4">
-        <v>4.5492336894285224E-2</v>
-      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2041</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="5">
         <v>0.03</v>
       </c>
-      <c r="C22" s="4">
-        <v>0.23062618419074904</v>
-      </c>
-      <c r="D22" s="4">
-        <v>4.8772746099148022E-2</v>
-      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2042</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>2.6666666666666665E-2</v>
       </c>
-      <c r="C23" s="5">
-        <v>0.20500105261399915</v>
-      </c>
-      <c r="D23" s="4">
-        <v>3.0256374903294497E-2</v>
-      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2043</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="6">
         <v>2.3333333333333331E-2</v>
       </c>
-      <c r="C24" s="5">
-        <v>0.17937592103724925</v>
-      </c>
-      <c r="D24" s="4">
-        <v>2.6474328040382685E-2</v>
-      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2044</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="6">
         <v>1.9999999999999997E-2</v>
       </c>
-      <c r="C25" s="5">
-        <v>0.15375078946049936</v>
-      </c>
-      <c r="D25" s="4">
-        <v>2.2692281177470873E-2</v>
-      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2045</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="6">
         <v>1.6666666666666663E-2</v>
       </c>
-      <c r="C26" s="5">
-        <v>0.12812565788374947</v>
-      </c>
-      <c r="D26" s="4">
-        <v>1.8910234314559061E-2</v>
-      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2046</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="6">
         <v>1.3333333333333329E-2</v>
       </c>
-      <c r="C27" s="5">
-        <v>0.10250052630699957</v>
-      </c>
-      <c r="D27" s="4">
-        <v>1.5128187451647249E-2</v>
-      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2047</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="6">
         <v>9.999999999999995E-3</v>
       </c>
-      <c r="C28" s="5">
-        <v>7.687539473024968E-2</v>
-      </c>
-      <c r="D28" s="4">
-        <v>1.1346140588735436E-2</v>
-      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2048</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="6">
         <v>6.6666666666666619E-3</v>
       </c>
-      <c r="C29" s="5">
-        <v>5.1250263153499787E-2</v>
-      </c>
-      <c r="D29" s="4">
-        <v>7.5640937258236243E-3</v>
-      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2049</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="6">
         <v>3.3333333333333288E-3</v>
       </c>
-      <c r="C30" s="5">
-        <v>2.5625131576749893E-2</v>
-      </c>
-      <c r="D30" s="4">
-        <v>3.7820468629118122E-3</v>
-      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2050</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="6">
         <v>0</v>
       </c>
-      <c r="C31" s="5">
-        <v>0</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0</v>
-      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C32" s="1"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>